<commit_message>
trying out a different way
</commit_message>
<xml_diff>
--- a/borders.xlsx
+++ b/borders.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="76">
   <si>
     <t>Algeria</t>
   </si>
@@ -228,6 +228,30 @@
   </si>
   <si>
     <t>Congo River</t>
+  </si>
+  <si>
+    <t>Nairobi</t>
+  </si>
+  <si>
+    <t>Kampala</t>
+  </si>
+  <si>
+    <t>Africa - South</t>
+  </si>
+  <si>
+    <t>Harare</t>
+  </si>
+  <si>
+    <t>White Nile</t>
+  </si>
+  <si>
+    <t>Lake Tanganyika</t>
+  </si>
+  <si>
+    <t>Lake Albert</t>
+  </si>
+  <si>
+    <t>Benghazi</t>
   </si>
 </sst>
 </file>
@@ -552,13 +576,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BP68"/>
+  <dimension ref="A1:BX76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AM13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BP14" sqref="BP14"/>
+      <selection pane="bottomRight" activeCell="AO30" sqref="AO30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -567,9 +591,10 @@
     <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -774,8 +799,32 @@
       <c r="BP1" t="s">
         <v>67</v>
       </c>
+      <c r="BQ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -980,8 +1029,32 @@
       <c r="BP2">
         <v>0</v>
       </c>
+      <c r="BQ2">
+        <v>0</v>
+      </c>
+      <c r="BR2">
+        <v>0</v>
+      </c>
+      <c r="BS2">
+        <v>0</v>
+      </c>
+      <c r="BT2">
+        <v>0</v>
+      </c>
+      <c r="BU2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BW2">
+        <v>0</v>
+      </c>
+      <c r="BX2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1186,8 +1259,32 @@
       <c r="BP3">
         <v>0</v>
       </c>
+      <c r="BQ3">
+        <v>0</v>
+      </c>
+      <c r="BR3">
+        <v>0</v>
+      </c>
+      <c r="BS3">
+        <v>1</v>
+      </c>
+      <c r="BT3">
+        <v>0</v>
+      </c>
+      <c r="BU3">
+        <v>0</v>
+      </c>
+      <c r="BV3">
+        <v>0</v>
+      </c>
+      <c r="BW3">
+        <v>0</v>
+      </c>
+      <c r="BX3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1392,8 +1489,32 @@
       <c r="BP4">
         <v>0</v>
       </c>
+      <c r="BQ4">
+        <v>0</v>
+      </c>
+      <c r="BR4">
+        <v>0</v>
+      </c>
+      <c r="BS4">
+        <v>0</v>
+      </c>
+      <c r="BT4">
+        <v>0</v>
+      </c>
+      <c r="BU4">
+        <v>0</v>
+      </c>
+      <c r="BV4">
+        <v>0</v>
+      </c>
+      <c r="BW4">
+        <v>0</v>
+      </c>
+      <c r="BX4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1455,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1598,8 +1719,32 @@
       <c r="BP5">
         <v>0</v>
       </c>
+      <c r="BQ5">
+        <v>0</v>
+      </c>
+      <c r="BR5">
+        <v>0</v>
+      </c>
+      <c r="BS5">
+        <v>0</v>
+      </c>
+      <c r="BT5">
+        <v>0</v>
+      </c>
+      <c r="BU5">
+        <v>1</v>
+      </c>
+      <c r="BV5">
+        <v>0</v>
+      </c>
+      <c r="BW5">
+        <v>0</v>
+      </c>
+      <c r="BX5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1804,8 +1949,32 @@
       <c r="BP6">
         <v>0</v>
       </c>
+      <c r="BQ6">
+        <v>0</v>
+      </c>
+      <c r="BR6">
+        <v>0</v>
+      </c>
+      <c r="BS6">
+        <v>0</v>
+      </c>
+      <c r="BT6">
+        <v>0</v>
+      </c>
+      <c r="BU6">
+        <v>0</v>
+      </c>
+      <c r="BV6">
+        <v>0</v>
+      </c>
+      <c r="BW6">
+        <v>0</v>
+      </c>
+      <c r="BX6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2010,8 +2179,32 @@
       <c r="BP7">
         <v>0</v>
       </c>
+      <c r="BQ7">
+        <v>0</v>
+      </c>
+      <c r="BR7">
+        <v>0</v>
+      </c>
+      <c r="BS7">
+        <v>0</v>
+      </c>
+      <c r="BT7">
+        <v>0</v>
+      </c>
+      <c r="BU7">
+        <v>0</v>
+      </c>
+      <c r="BV7">
+        <v>0</v>
+      </c>
+      <c r="BW7">
+        <v>0</v>
+      </c>
+      <c r="BX7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2216,8 +2409,32 @@
       <c r="BP8">
         <v>0</v>
       </c>
+      <c r="BQ8">
+        <v>0</v>
+      </c>
+      <c r="BR8">
+        <v>0</v>
+      </c>
+      <c r="BS8">
+        <v>0</v>
+      </c>
+      <c r="BT8">
+        <v>0</v>
+      </c>
+      <c r="BU8">
+        <v>0</v>
+      </c>
+      <c r="BV8">
+        <v>0</v>
+      </c>
+      <c r="BW8">
+        <v>0</v>
+      </c>
+      <c r="BX8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2422,8 +2639,32 @@
       <c r="BP9">
         <v>0</v>
       </c>
+      <c r="BQ9">
+        <v>0</v>
+      </c>
+      <c r="BR9">
+        <v>0</v>
+      </c>
+      <c r="BS9">
+        <v>0</v>
+      </c>
+      <c r="BT9">
+        <v>0</v>
+      </c>
+      <c r="BU9">
+        <v>0</v>
+      </c>
+      <c r="BV9">
+        <v>0</v>
+      </c>
+      <c r="BW9">
+        <v>0</v>
+      </c>
+      <c r="BX9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2628,8 +2869,32 @@
       <c r="BP10">
         <v>0</v>
       </c>
+      <c r="BQ10">
+        <v>0</v>
+      </c>
+      <c r="BR10">
+        <v>0</v>
+      </c>
+      <c r="BS10">
+        <v>0</v>
+      </c>
+      <c r="BT10">
+        <v>0</v>
+      </c>
+      <c r="BU10">
+        <v>0</v>
+      </c>
+      <c r="BV10">
+        <v>0</v>
+      </c>
+      <c r="BW10">
+        <v>0</v>
+      </c>
+      <c r="BX10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2834,8 +3099,32 @@
       <c r="BP11">
         <v>0</v>
       </c>
+      <c r="BQ11">
+        <v>0</v>
+      </c>
+      <c r="BR11">
+        <v>0</v>
+      </c>
+      <c r="BS11">
+        <v>0</v>
+      </c>
+      <c r="BT11">
+        <v>0</v>
+      </c>
+      <c r="BU11">
+        <v>0</v>
+      </c>
+      <c r="BV11">
+        <v>0</v>
+      </c>
+      <c r="BW11">
+        <v>0</v>
+      </c>
+      <c r="BX11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3040,8 +3329,32 @@
       <c r="BP12">
         <v>0</v>
       </c>
+      <c r="BQ12">
+        <v>0</v>
+      </c>
+      <c r="BR12">
+        <v>0</v>
+      </c>
+      <c r="BS12">
+        <v>0</v>
+      </c>
+      <c r="BT12">
+        <v>0</v>
+      </c>
+      <c r="BU12">
+        <v>0</v>
+      </c>
+      <c r="BV12">
+        <v>0</v>
+      </c>
+      <c r="BW12">
+        <v>0</v>
+      </c>
+      <c r="BX12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3246,8 +3559,32 @@
       <c r="BP13">
         <v>0</v>
       </c>
+      <c r="BQ13">
+        <v>0</v>
+      </c>
+      <c r="BR13">
+        <v>0</v>
+      </c>
+      <c r="BS13">
+        <v>0</v>
+      </c>
+      <c r="BT13">
+        <v>0</v>
+      </c>
+      <c r="BU13">
+        <v>0</v>
+      </c>
+      <c r="BV13">
+        <v>0</v>
+      </c>
+      <c r="BW13">
+        <v>0</v>
+      </c>
+      <c r="BX13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3452,8 +3789,32 @@
       <c r="BP14">
         <v>0</v>
       </c>
+      <c r="BQ14">
+        <v>0</v>
+      </c>
+      <c r="BR14">
+        <v>0</v>
+      </c>
+      <c r="BS14">
+        <v>0</v>
+      </c>
+      <c r="BT14">
+        <v>0</v>
+      </c>
+      <c r="BU14">
+        <v>0</v>
+      </c>
+      <c r="BV14">
+        <v>0</v>
+      </c>
+      <c r="BW14">
+        <v>0</v>
+      </c>
+      <c r="BX14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3658,8 +4019,32 @@
       <c r="BP15">
         <v>1</v>
       </c>
+      <c r="BQ15">
+        <v>0</v>
+      </c>
+      <c r="BR15">
+        <v>0</v>
+      </c>
+      <c r="BS15">
+        <v>0</v>
+      </c>
+      <c r="BT15">
+        <v>0</v>
+      </c>
+      <c r="BU15">
+        <v>0</v>
+      </c>
+      <c r="BV15">
+        <v>0</v>
+      </c>
+      <c r="BW15">
+        <v>0</v>
+      </c>
+      <c r="BX15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3864,8 +4249,32 @@
       <c r="BP16">
         <v>0</v>
       </c>
+      <c r="BQ16">
+        <v>0</v>
+      </c>
+      <c r="BR16">
+        <v>0</v>
+      </c>
+      <c r="BS16">
+        <v>0</v>
+      </c>
+      <c r="BT16">
+        <v>0</v>
+      </c>
+      <c r="BU16">
+        <v>0</v>
+      </c>
+      <c r="BV16">
+        <v>0</v>
+      </c>
+      <c r="BW16">
+        <v>0</v>
+      </c>
+      <c r="BX16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -4070,8 +4479,32 @@
       <c r="BP17">
         <v>0</v>
       </c>
+      <c r="BQ17">
+        <v>0</v>
+      </c>
+      <c r="BR17">
+        <v>0</v>
+      </c>
+      <c r="BS17">
+        <v>0</v>
+      </c>
+      <c r="BT17">
+        <v>0</v>
+      </c>
+      <c r="BU17">
+        <v>0</v>
+      </c>
+      <c r="BV17">
+        <v>0</v>
+      </c>
+      <c r="BW17">
+        <v>0</v>
+      </c>
+      <c r="BX17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -4276,8 +4709,32 @@
       <c r="BP18">
         <v>0</v>
       </c>
+      <c r="BQ18">
+        <v>0</v>
+      </c>
+      <c r="BR18">
+        <v>0</v>
+      </c>
+      <c r="BS18">
+        <v>0</v>
+      </c>
+      <c r="BT18">
+        <v>0</v>
+      </c>
+      <c r="BU18">
+        <v>0</v>
+      </c>
+      <c r="BV18">
+        <v>0</v>
+      </c>
+      <c r="BW18">
+        <v>0</v>
+      </c>
+      <c r="BX18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -4477,13 +4934,37 @@
         <v>0</v>
       </c>
       <c r="BO19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP19">
         <v>0</v>
       </c>
+      <c r="BQ19">
+        <v>0</v>
+      </c>
+      <c r="BR19">
+        <v>0</v>
+      </c>
+      <c r="BS19">
+        <v>0</v>
+      </c>
+      <c r="BT19">
+        <v>0</v>
+      </c>
+      <c r="BU19">
+        <v>0</v>
+      </c>
+      <c r="BV19">
+        <v>0</v>
+      </c>
+      <c r="BW19">
+        <v>0</v>
+      </c>
+      <c r="BX19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -4688,8 +5169,32 @@
       <c r="BP20">
         <v>0</v>
       </c>
+      <c r="BQ20">
+        <v>0</v>
+      </c>
+      <c r="BR20">
+        <v>0</v>
+      </c>
+      <c r="BS20">
+        <v>0</v>
+      </c>
+      <c r="BT20">
+        <v>0</v>
+      </c>
+      <c r="BU20">
+        <v>0</v>
+      </c>
+      <c r="BV20">
+        <v>0</v>
+      </c>
+      <c r="BW20">
+        <v>0</v>
+      </c>
+      <c r="BX20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -4894,8 +5399,32 @@
       <c r="BP21">
         <v>0</v>
       </c>
+      <c r="BQ21">
+        <v>0</v>
+      </c>
+      <c r="BR21">
+        <v>0</v>
+      </c>
+      <c r="BS21">
+        <v>0</v>
+      </c>
+      <c r="BT21">
+        <v>0</v>
+      </c>
+      <c r="BU21">
+        <v>0</v>
+      </c>
+      <c r="BV21">
+        <v>0</v>
+      </c>
+      <c r="BW21">
+        <v>0</v>
+      </c>
+      <c r="BX21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -5100,8 +5629,32 @@
       <c r="BP22">
         <v>0</v>
       </c>
+      <c r="BQ22">
+        <v>0</v>
+      </c>
+      <c r="BR22">
+        <v>0</v>
+      </c>
+      <c r="BS22">
+        <v>0</v>
+      </c>
+      <c r="BT22">
+        <v>0</v>
+      </c>
+      <c r="BU22">
+        <v>0</v>
+      </c>
+      <c r="BV22">
+        <v>0</v>
+      </c>
+      <c r="BW22">
+        <v>0</v>
+      </c>
+      <c r="BX22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -5306,8 +5859,32 @@
       <c r="BP23">
         <v>0</v>
       </c>
+      <c r="BQ23">
+        <v>0</v>
+      </c>
+      <c r="BR23">
+        <v>0</v>
+      </c>
+      <c r="BS23">
+        <v>0</v>
+      </c>
+      <c r="BT23">
+        <v>0</v>
+      </c>
+      <c r="BU23">
+        <v>0</v>
+      </c>
+      <c r="BV23">
+        <v>0</v>
+      </c>
+      <c r="BW23">
+        <v>0</v>
+      </c>
+      <c r="BX23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -5512,8 +6089,32 @@
       <c r="BP24">
         <v>0</v>
       </c>
+      <c r="BQ24">
+        <v>0</v>
+      </c>
+      <c r="BR24">
+        <v>0</v>
+      </c>
+      <c r="BS24">
+        <v>0</v>
+      </c>
+      <c r="BT24">
+        <v>0</v>
+      </c>
+      <c r="BU24">
+        <v>0</v>
+      </c>
+      <c r="BV24">
+        <v>0</v>
+      </c>
+      <c r="BW24">
+        <v>0</v>
+      </c>
+      <c r="BX24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -5718,8 +6319,32 @@
       <c r="BP25">
         <v>0</v>
       </c>
+      <c r="BQ25">
+        <v>0</v>
+      </c>
+      <c r="BR25">
+        <v>0</v>
+      </c>
+      <c r="BS25">
+        <v>0</v>
+      </c>
+      <c r="BT25">
+        <v>0</v>
+      </c>
+      <c r="BU25">
+        <v>0</v>
+      </c>
+      <c r="BV25">
+        <v>0</v>
+      </c>
+      <c r="BW25">
+        <v>0</v>
+      </c>
+      <c r="BX25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -5924,8 +6549,32 @@
       <c r="BP26">
         <v>0</v>
       </c>
+      <c r="BQ26">
+        <v>0</v>
+      </c>
+      <c r="BR26">
+        <v>0</v>
+      </c>
+      <c r="BS26">
+        <v>0</v>
+      </c>
+      <c r="BT26">
+        <v>0</v>
+      </c>
+      <c r="BU26">
+        <v>0</v>
+      </c>
+      <c r="BV26">
+        <v>0</v>
+      </c>
+      <c r="BW26">
+        <v>0</v>
+      </c>
+      <c r="BX26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -6130,8 +6779,32 @@
       <c r="BP27">
         <v>0</v>
       </c>
+      <c r="BQ27">
+        <v>1</v>
+      </c>
+      <c r="BR27">
+        <v>0</v>
+      </c>
+      <c r="BS27">
+        <v>0</v>
+      </c>
+      <c r="BT27">
+        <v>0</v>
+      </c>
+      <c r="BU27">
+        <v>0</v>
+      </c>
+      <c r="BV27">
+        <v>0</v>
+      </c>
+      <c r="BW27">
+        <v>0</v>
+      </c>
+      <c r="BX27">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -6336,8 +7009,32 @@
       <c r="BP28">
         <v>0</v>
       </c>
+      <c r="BQ28">
+        <v>0</v>
+      </c>
+      <c r="BR28">
+        <v>0</v>
+      </c>
+      <c r="BS28">
+        <v>0</v>
+      </c>
+      <c r="BT28">
+        <v>0</v>
+      </c>
+      <c r="BU28">
+        <v>1</v>
+      </c>
+      <c r="BV28">
+        <v>0</v>
+      </c>
+      <c r="BW28">
+        <v>0</v>
+      </c>
+      <c r="BX28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -6399,7 +7096,7 @@
         <v>0</v>
       </c>
       <c r="U29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V29">
         <v>0</v>
@@ -6542,8 +7239,32 @@
       <c r="BP29">
         <v>0</v>
       </c>
+      <c r="BQ29">
+        <v>0</v>
+      </c>
+      <c r="BR29">
+        <v>0</v>
+      </c>
+      <c r="BS29">
+        <v>0</v>
+      </c>
+      <c r="BT29">
+        <v>0</v>
+      </c>
+      <c r="BU29">
+        <v>1</v>
+      </c>
+      <c r="BV29">
+        <v>0</v>
+      </c>
+      <c r="BW29">
+        <v>0</v>
+      </c>
+      <c r="BX29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -6748,8 +7469,32 @@
       <c r="BP30">
         <v>0</v>
       </c>
+      <c r="BQ30">
+        <v>0</v>
+      </c>
+      <c r="BR30">
+        <v>1</v>
+      </c>
+      <c r="BS30">
+        <v>0</v>
+      </c>
+      <c r="BT30">
+        <v>0</v>
+      </c>
+      <c r="BU30">
+        <v>1</v>
+      </c>
+      <c r="BV30">
+        <v>1</v>
+      </c>
+      <c r="BW30">
+        <v>1</v>
+      </c>
+      <c r="BX30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -6871,7 +7616,7 @@
         <v>0</v>
       </c>
       <c r="AO31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP31">
         <v>0</v>
@@ -6954,8 +7699,32 @@
       <c r="BP31">
         <v>0</v>
       </c>
+      <c r="BQ31">
+        <v>0</v>
+      </c>
+      <c r="BR31">
+        <v>0</v>
+      </c>
+      <c r="BS31">
+        <v>0</v>
+      </c>
+      <c r="BT31">
+        <v>0</v>
+      </c>
+      <c r="BU31">
+        <v>0</v>
+      </c>
+      <c r="BV31">
+        <v>0</v>
+      </c>
+      <c r="BW31">
+        <v>0</v>
+      </c>
+      <c r="BX31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -7107,7 +7876,7 @@
         <v>0</v>
       </c>
       <c r="AY32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ32">
         <v>0</v>
@@ -7160,8 +7929,32 @@
       <c r="BP32">
         <v>0</v>
       </c>
+      <c r="BQ32">
+        <v>0</v>
+      </c>
+      <c r="BR32">
+        <v>0</v>
+      </c>
+      <c r="BS32">
+        <v>0</v>
+      </c>
+      <c r="BT32">
+        <v>0</v>
+      </c>
+      <c r="BU32">
+        <v>0</v>
+      </c>
+      <c r="BV32">
+        <v>0</v>
+      </c>
+      <c r="BW32">
+        <v>0</v>
+      </c>
+      <c r="BX32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -7328,7 +8121,7 @@
         <v>0</v>
       </c>
       <c r="BD33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE33">
         <v>0</v>
@@ -7366,8 +8159,32 @@
       <c r="BP33">
         <v>0</v>
       </c>
+      <c r="BQ33">
+        <v>0</v>
+      </c>
+      <c r="BR33">
+        <v>0</v>
+      </c>
+      <c r="BS33">
+        <v>0</v>
+      </c>
+      <c r="BT33">
+        <v>0</v>
+      </c>
+      <c r="BU33">
+        <v>0</v>
+      </c>
+      <c r="BV33">
+        <v>0</v>
+      </c>
+      <c r="BW33">
+        <v>0</v>
+      </c>
+      <c r="BX33">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -7572,8 +8389,32 @@
       <c r="BP34">
         <v>0</v>
       </c>
+      <c r="BQ34">
+        <v>0</v>
+      </c>
+      <c r="BR34">
+        <v>0</v>
+      </c>
+      <c r="BS34">
+        <v>0</v>
+      </c>
+      <c r="BT34">
+        <v>0</v>
+      </c>
+      <c r="BU34">
+        <v>0</v>
+      </c>
+      <c r="BV34">
+        <v>0</v>
+      </c>
+      <c r="BW34">
+        <v>0</v>
+      </c>
+      <c r="BX34">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -7778,8 +8619,32 @@
       <c r="BP35">
         <v>0</v>
       </c>
+      <c r="BQ35">
+        <v>0</v>
+      </c>
+      <c r="BR35">
+        <v>0</v>
+      </c>
+      <c r="BS35">
+        <v>0</v>
+      </c>
+      <c r="BT35">
+        <v>0</v>
+      </c>
+      <c r="BU35">
+        <v>0</v>
+      </c>
+      <c r="BV35">
+        <v>0</v>
+      </c>
+      <c r="BW35">
+        <v>0</v>
+      </c>
+      <c r="BX35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -7984,8 +8849,32 @@
       <c r="BP36">
         <v>0</v>
       </c>
+      <c r="BQ36">
+        <v>0</v>
+      </c>
+      <c r="BR36">
+        <v>0</v>
+      </c>
+      <c r="BS36">
+        <v>0</v>
+      </c>
+      <c r="BT36">
+        <v>0</v>
+      </c>
+      <c r="BU36">
+        <v>0</v>
+      </c>
+      <c r="BV36">
+        <v>0</v>
+      </c>
+      <c r="BW36">
+        <v>0</v>
+      </c>
+      <c r="BX36">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -8190,8 +9079,32 @@
       <c r="BP37">
         <v>0</v>
       </c>
+      <c r="BQ37">
+        <v>0</v>
+      </c>
+      <c r="BR37">
+        <v>0</v>
+      </c>
+      <c r="BS37">
+        <v>0</v>
+      </c>
+      <c r="BT37">
+        <v>0</v>
+      </c>
+      <c r="BU37">
+        <v>0</v>
+      </c>
+      <c r="BV37">
+        <v>0</v>
+      </c>
+      <c r="BW37">
+        <v>0</v>
+      </c>
+      <c r="BX37">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -8396,8 +9309,32 @@
       <c r="BP38">
         <v>0</v>
       </c>
+      <c r="BQ38">
+        <v>0</v>
+      </c>
+      <c r="BR38">
+        <v>0</v>
+      </c>
+      <c r="BS38">
+        <v>0</v>
+      </c>
+      <c r="BT38">
+        <v>0</v>
+      </c>
+      <c r="BU38">
+        <v>0</v>
+      </c>
+      <c r="BV38">
+        <v>0</v>
+      </c>
+      <c r="BW38">
+        <v>0</v>
+      </c>
+      <c r="BX38">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -8602,8 +9539,32 @@
       <c r="BP39">
         <v>0</v>
       </c>
+      <c r="BQ39">
+        <v>0</v>
+      </c>
+      <c r="BR39">
+        <v>0</v>
+      </c>
+      <c r="BS39">
+        <v>0</v>
+      </c>
+      <c r="BT39">
+        <v>0</v>
+      </c>
+      <c r="BU39">
+        <v>0</v>
+      </c>
+      <c r="BV39">
+        <v>0</v>
+      </c>
+      <c r="BW39">
+        <v>0</v>
+      </c>
+      <c r="BX39">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -8808,8 +9769,32 @@
       <c r="BP40">
         <v>0</v>
       </c>
+      <c r="BQ40">
+        <v>0</v>
+      </c>
+      <c r="BR40">
+        <v>0</v>
+      </c>
+      <c r="BS40">
+        <v>0</v>
+      </c>
+      <c r="BT40">
+        <v>0</v>
+      </c>
+      <c r="BU40">
+        <v>0</v>
+      </c>
+      <c r="BV40">
+        <v>0</v>
+      </c>
+      <c r="BW40">
+        <v>0</v>
+      </c>
+      <c r="BX40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -9014,8 +9999,32 @@
       <c r="BP41">
         <v>0</v>
       </c>
+      <c r="BQ41">
+        <v>0</v>
+      </c>
+      <c r="BR41">
+        <v>0</v>
+      </c>
+      <c r="BS41">
+        <v>1</v>
+      </c>
+      <c r="BT41">
+        <v>0</v>
+      </c>
+      <c r="BU41">
+        <v>0</v>
+      </c>
+      <c r="BV41">
+        <v>0</v>
+      </c>
+      <c r="BW41">
+        <v>0</v>
+      </c>
+      <c r="BX41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -9220,8 +10229,32 @@
       <c r="BP42">
         <v>0</v>
       </c>
+      <c r="BQ42">
+        <v>0</v>
+      </c>
+      <c r="BR42">
+        <v>0</v>
+      </c>
+      <c r="BS42">
+        <v>0</v>
+      </c>
+      <c r="BT42">
+        <v>0</v>
+      </c>
+      <c r="BU42">
+        <v>0</v>
+      </c>
+      <c r="BV42">
+        <v>0</v>
+      </c>
+      <c r="BW42">
+        <v>0</v>
+      </c>
+      <c r="BX42">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -9426,8 +10459,32 @@
       <c r="BP43">
         <v>0</v>
       </c>
+      <c r="BQ43">
+        <v>0</v>
+      </c>
+      <c r="BR43">
+        <v>0</v>
+      </c>
+      <c r="BS43">
+        <v>0</v>
+      </c>
+      <c r="BT43">
+        <v>0</v>
+      </c>
+      <c r="BU43">
+        <v>0</v>
+      </c>
+      <c r="BV43">
+        <v>0</v>
+      </c>
+      <c r="BW43">
+        <v>0</v>
+      </c>
+      <c r="BX43">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -9632,8 +10689,32 @@
       <c r="BP44">
         <v>0</v>
       </c>
+      <c r="BQ44">
+        <v>0</v>
+      </c>
+      <c r="BR44">
+        <v>0</v>
+      </c>
+      <c r="BS44">
+        <v>0</v>
+      </c>
+      <c r="BT44">
+        <v>0</v>
+      </c>
+      <c r="BU44">
+        <v>0</v>
+      </c>
+      <c r="BV44">
+        <v>0</v>
+      </c>
+      <c r="BW44">
+        <v>0</v>
+      </c>
+      <c r="BX44">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -9838,8 +10919,32 @@
       <c r="BP45">
         <v>0</v>
       </c>
+      <c r="BQ45">
+        <v>0</v>
+      </c>
+      <c r="BR45">
+        <v>0</v>
+      </c>
+      <c r="BS45">
+        <v>0</v>
+      </c>
+      <c r="BT45">
+        <v>0</v>
+      </c>
+      <c r="BU45">
+        <v>0</v>
+      </c>
+      <c r="BV45">
+        <v>0</v>
+      </c>
+      <c r="BW45">
+        <v>0</v>
+      </c>
+      <c r="BX45">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -10044,8 +11149,32 @@
       <c r="BP46">
         <v>0</v>
       </c>
+      <c r="BQ46">
+        <v>0</v>
+      </c>
+      <c r="BR46">
+        <v>0</v>
+      </c>
+      <c r="BS46">
+        <v>0</v>
+      </c>
+      <c r="BT46">
+        <v>0</v>
+      </c>
+      <c r="BU46">
+        <v>0</v>
+      </c>
+      <c r="BV46">
+        <v>0</v>
+      </c>
+      <c r="BW46">
+        <v>0</v>
+      </c>
+      <c r="BX46">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -10250,8 +11379,32 @@
       <c r="BP47">
         <v>0</v>
       </c>
+      <c r="BQ47">
+        <v>0</v>
+      </c>
+      <c r="BR47">
+        <v>0</v>
+      </c>
+      <c r="BS47">
+        <v>0</v>
+      </c>
+      <c r="BT47">
+        <v>0</v>
+      </c>
+      <c r="BU47">
+        <v>0</v>
+      </c>
+      <c r="BV47">
+        <v>0</v>
+      </c>
+      <c r="BW47">
+        <v>0</v>
+      </c>
+      <c r="BX47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -10456,8 +11609,32 @@
       <c r="BP48">
         <v>0</v>
       </c>
+      <c r="BQ48">
+        <v>0</v>
+      </c>
+      <c r="BR48">
+        <v>0</v>
+      </c>
+      <c r="BS48">
+        <v>0</v>
+      </c>
+      <c r="BT48">
+        <v>0</v>
+      </c>
+      <c r="BU48">
+        <v>0</v>
+      </c>
+      <c r="BV48">
+        <v>0</v>
+      </c>
+      <c r="BW48">
+        <v>0</v>
+      </c>
+      <c r="BX48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -10662,8 +11839,32 @@
       <c r="BP49">
         <v>0</v>
       </c>
+      <c r="BQ49">
+        <v>0</v>
+      </c>
+      <c r="BR49">
+        <v>0</v>
+      </c>
+      <c r="BS49">
+        <v>0</v>
+      </c>
+      <c r="BT49">
+        <v>0</v>
+      </c>
+      <c r="BU49">
+        <v>0</v>
+      </c>
+      <c r="BV49">
+        <v>0</v>
+      </c>
+      <c r="BW49">
+        <v>0</v>
+      </c>
+      <c r="BX49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -10868,8 +12069,32 @@
       <c r="BP50">
         <v>0</v>
       </c>
+      <c r="BQ50">
+        <v>0</v>
+      </c>
+      <c r="BR50">
+        <v>0</v>
+      </c>
+      <c r="BS50">
+        <v>0</v>
+      </c>
+      <c r="BT50">
+        <v>0</v>
+      </c>
+      <c r="BU50">
+        <v>0</v>
+      </c>
+      <c r="BV50">
+        <v>0</v>
+      </c>
+      <c r="BW50">
+        <v>0</v>
+      </c>
+      <c r="BX50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -11074,8 +12299,32 @@
       <c r="BP51">
         <v>0</v>
       </c>
+      <c r="BQ51">
+        <v>0</v>
+      </c>
+      <c r="BR51">
+        <v>0</v>
+      </c>
+      <c r="BS51">
+        <v>0</v>
+      </c>
+      <c r="BT51">
+        <v>0</v>
+      </c>
+      <c r="BU51">
+        <v>0</v>
+      </c>
+      <c r="BV51">
+        <v>0</v>
+      </c>
+      <c r="BW51">
+        <v>0</v>
+      </c>
+      <c r="BX51">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -11233,7 +12482,7 @@
         <v>0</v>
       </c>
       <c r="BA52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB52">
         <v>0</v>
@@ -11280,8 +12529,32 @@
       <c r="BP52">
         <v>0</v>
       </c>
+      <c r="BQ52">
+        <v>0</v>
+      </c>
+      <c r="BR52">
+        <v>0</v>
+      </c>
+      <c r="BS52">
+        <v>0</v>
+      </c>
+      <c r="BT52">
+        <v>0</v>
+      </c>
+      <c r="BU52">
+        <v>0</v>
+      </c>
+      <c r="BV52">
+        <v>0</v>
+      </c>
+      <c r="BW52">
+        <v>0</v>
+      </c>
+      <c r="BX52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -11436,7 +12709,7 @@
         <v>0</v>
       </c>
       <c r="AZ53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA53">
         <v>0</v>
@@ -11486,8 +12759,32 @@
       <c r="BP53">
         <v>0</v>
       </c>
+      <c r="BQ53">
+        <v>0</v>
+      </c>
+      <c r="BR53">
+        <v>0</v>
+      </c>
+      <c r="BS53">
+        <v>0</v>
+      </c>
+      <c r="BT53">
+        <v>0</v>
+      </c>
+      <c r="BU53">
+        <v>0</v>
+      </c>
+      <c r="BV53">
+        <v>0</v>
+      </c>
+      <c r="BW53">
+        <v>0</v>
+      </c>
+      <c r="BX53">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -11692,8 +12989,32 @@
       <c r="BP54">
         <v>0</v>
       </c>
+      <c r="BQ54">
+        <v>0</v>
+      </c>
+      <c r="BR54">
+        <v>0</v>
+      </c>
+      <c r="BS54">
+        <v>0</v>
+      </c>
+      <c r="BT54">
+        <v>0</v>
+      </c>
+      <c r="BU54">
+        <v>0</v>
+      </c>
+      <c r="BV54">
+        <v>0</v>
+      </c>
+      <c r="BW54">
+        <v>0</v>
+      </c>
+      <c r="BX54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -11860,7 +13181,7 @@
         <v>0</v>
       </c>
       <c r="BD55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE55">
         <v>0</v>
@@ -11898,8 +13219,32 @@
       <c r="BP55">
         <v>0</v>
       </c>
+      <c r="BQ55">
+        <v>0</v>
+      </c>
+      <c r="BR55">
+        <v>0</v>
+      </c>
+      <c r="BS55">
+        <v>0</v>
+      </c>
+      <c r="BT55">
+        <v>0</v>
+      </c>
+      <c r="BU55">
+        <v>0</v>
+      </c>
+      <c r="BV55">
+        <v>0</v>
+      </c>
+      <c r="BW55">
+        <v>0</v>
+      </c>
+      <c r="BX55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -12099,13 +13444,37 @@
         <v>0</v>
       </c>
       <c r="BO56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP56">
         <v>0</v>
       </c>
+      <c r="BQ56">
+        <v>0</v>
+      </c>
+      <c r="BR56">
+        <v>0</v>
+      </c>
+      <c r="BS56">
+        <v>0</v>
+      </c>
+      <c r="BT56">
+        <v>0</v>
+      </c>
+      <c r="BU56">
+        <v>0</v>
+      </c>
+      <c r="BV56">
+        <v>0</v>
+      </c>
+      <c r="BW56">
+        <v>0</v>
+      </c>
+      <c r="BX56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -12310,8 +13679,32 @@
       <c r="BP57">
         <v>0</v>
       </c>
+      <c r="BQ57">
+        <v>0</v>
+      </c>
+      <c r="BR57">
+        <v>0</v>
+      </c>
+      <c r="BS57">
+        <v>0</v>
+      </c>
+      <c r="BT57">
+        <v>0</v>
+      </c>
+      <c r="BU57">
+        <v>0</v>
+      </c>
+      <c r="BV57">
+        <v>0</v>
+      </c>
+      <c r="BW57">
+        <v>0</v>
+      </c>
+      <c r="BX57">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -12516,8 +13909,32 @@
       <c r="BP58">
         <v>0</v>
       </c>
+      <c r="BQ58">
+        <v>0</v>
+      </c>
+      <c r="BR58">
+        <v>0</v>
+      </c>
+      <c r="BS58">
+        <v>0</v>
+      </c>
+      <c r="BT58">
+        <v>0</v>
+      </c>
+      <c r="BU58">
+        <v>0</v>
+      </c>
+      <c r="BV58">
+        <v>1</v>
+      </c>
+      <c r="BW58">
+        <v>0</v>
+      </c>
+      <c r="BX58">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -12722,8 +14139,32 @@
       <c r="BP59">
         <v>0</v>
       </c>
+      <c r="BQ59">
+        <v>0</v>
+      </c>
+      <c r="BR59">
+        <v>0</v>
+      </c>
+      <c r="BS59">
+        <v>0</v>
+      </c>
+      <c r="BT59">
+        <v>0</v>
+      </c>
+      <c r="BU59">
+        <v>0</v>
+      </c>
+      <c r="BV59">
+        <v>0</v>
+      </c>
+      <c r="BW59">
+        <v>0</v>
+      </c>
+      <c r="BX59">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -12928,8 +14369,32 @@
       <c r="BP60">
         <v>0</v>
       </c>
+      <c r="BQ60">
+        <v>0</v>
+      </c>
+      <c r="BR60">
+        <v>0</v>
+      </c>
+      <c r="BS60">
+        <v>0</v>
+      </c>
+      <c r="BT60">
+        <v>0</v>
+      </c>
+      <c r="BU60">
+        <v>0</v>
+      </c>
+      <c r="BV60">
+        <v>0</v>
+      </c>
+      <c r="BW60">
+        <v>0</v>
+      </c>
+      <c r="BX60">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -13134,8 +14599,32 @@
       <c r="BP61">
         <v>0</v>
       </c>
+      <c r="BQ61">
+        <v>0</v>
+      </c>
+      <c r="BR61">
+        <v>0</v>
+      </c>
+      <c r="BS61">
+        <v>0</v>
+      </c>
+      <c r="BT61">
+        <v>0</v>
+      </c>
+      <c r="BU61">
+        <v>0</v>
+      </c>
+      <c r="BV61">
+        <v>0</v>
+      </c>
+      <c r="BW61">
+        <v>0</v>
+      </c>
+      <c r="BX61">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -13340,8 +14829,32 @@
       <c r="BP62">
         <v>0</v>
       </c>
+      <c r="BQ62">
+        <v>0</v>
+      </c>
+      <c r="BR62">
+        <v>1</v>
+      </c>
+      <c r="BS62">
+        <v>0</v>
+      </c>
+      <c r="BT62">
+        <v>0</v>
+      </c>
+      <c r="BU62">
+        <v>0</v>
+      </c>
+      <c r="BV62">
+        <v>1</v>
+      </c>
+      <c r="BW62">
+        <v>0</v>
+      </c>
+      <c r="BX62">
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -13546,8 +15059,32 @@
       <c r="BP63">
         <v>0</v>
       </c>
+      <c r="BQ63">
+        <v>0</v>
+      </c>
+      <c r="BR63">
+        <v>0</v>
+      </c>
+      <c r="BS63">
+        <v>0</v>
+      </c>
+      <c r="BT63">
+        <v>0</v>
+      </c>
+      <c r="BU63">
+        <v>0</v>
+      </c>
+      <c r="BV63">
+        <v>0</v>
+      </c>
+      <c r="BW63">
+        <v>0</v>
+      </c>
+      <c r="BX63">
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -13752,8 +15289,32 @@
       <c r="BP64">
         <v>0</v>
       </c>
+      <c r="BQ64">
+        <v>0</v>
+      </c>
+      <c r="BR64">
+        <v>0</v>
+      </c>
+      <c r="BS64">
+        <v>0</v>
+      </c>
+      <c r="BT64">
+        <v>0</v>
+      </c>
+      <c r="BU64">
+        <v>0</v>
+      </c>
+      <c r="BV64">
+        <v>0</v>
+      </c>
+      <c r="BW64">
+        <v>0</v>
+      </c>
+      <c r="BX64">
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -13958,8 +15519,32 @@
       <c r="BP65">
         <v>0</v>
       </c>
+      <c r="BQ65">
+        <v>0</v>
+      </c>
+      <c r="BR65">
+        <v>0</v>
+      </c>
+      <c r="BS65">
+        <v>0</v>
+      </c>
+      <c r="BT65">
+        <v>1</v>
+      </c>
+      <c r="BU65">
+        <v>0</v>
+      </c>
+      <c r="BV65">
+        <v>0</v>
+      </c>
+      <c r="BW65">
+        <v>0</v>
+      </c>
+      <c r="BX65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -14164,8 +15749,32 @@
       <c r="BP66">
         <v>0</v>
       </c>
+      <c r="BQ66">
+        <v>0</v>
+      </c>
+      <c r="BR66">
+        <v>0</v>
+      </c>
+      <c r="BS66">
+        <v>0</v>
+      </c>
+      <c r="BT66">
+        <v>0</v>
+      </c>
+      <c r="BU66">
+        <v>0</v>
+      </c>
+      <c r="BV66">
+        <v>0</v>
+      </c>
+      <c r="BW66">
+        <v>0</v>
+      </c>
+      <c r="BX66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -14370,8 +15979,32 @@
       <c r="BP67">
         <v>0</v>
       </c>
+      <c r="BQ67">
+        <v>0</v>
+      </c>
+      <c r="BR67">
+        <v>0</v>
+      </c>
+      <c r="BS67">
+        <v>0</v>
+      </c>
+      <c r="BT67">
+        <v>0</v>
+      </c>
+      <c r="BU67">
+        <v>0</v>
+      </c>
+      <c r="BV67">
+        <v>0</v>
+      </c>
+      <c r="BW67">
+        <v>0</v>
+      </c>
+      <c r="BX67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -14574,6 +16207,1870 @@
         <v>0</v>
       </c>
       <c r="BP68">
+        <v>0</v>
+      </c>
+      <c r="BQ68">
+        <v>0</v>
+      </c>
+      <c r="BR68">
+        <v>0</v>
+      </c>
+      <c r="BS68">
+        <v>1</v>
+      </c>
+      <c r="BT68">
+        <v>0</v>
+      </c>
+      <c r="BU68">
+        <v>0</v>
+      </c>
+      <c r="BV68">
+        <v>0</v>
+      </c>
+      <c r="BW68">
+        <v>0</v>
+      </c>
+      <c r="BX68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <v>0</v>
+      </c>
+      <c r="S69">
+        <v>0</v>
+      </c>
+      <c r="T69">
+        <v>0</v>
+      </c>
+      <c r="U69">
+        <v>0</v>
+      </c>
+      <c r="V69">
+        <v>0</v>
+      </c>
+      <c r="W69">
+        <v>0</v>
+      </c>
+      <c r="X69">
+        <v>0</v>
+      </c>
+      <c r="Y69">
+        <v>0</v>
+      </c>
+      <c r="Z69">
+        <v>0</v>
+      </c>
+      <c r="AA69">
+        <v>0</v>
+      </c>
+      <c r="AB69">
+        <v>0</v>
+      </c>
+      <c r="AC69">
+        <v>0</v>
+      </c>
+      <c r="AD69">
+        <v>0</v>
+      </c>
+      <c r="AE69">
+        <v>0</v>
+      </c>
+      <c r="AF69">
+        <v>0</v>
+      </c>
+      <c r="AG69">
+        <v>0</v>
+      </c>
+      <c r="AH69">
+        <v>0</v>
+      </c>
+      <c r="AI69">
+        <v>0</v>
+      </c>
+      <c r="AJ69">
+        <v>0</v>
+      </c>
+      <c r="AK69">
+        <v>0</v>
+      </c>
+      <c r="AL69">
+        <v>0</v>
+      </c>
+      <c r="AM69">
+        <v>0</v>
+      </c>
+      <c r="AN69">
+        <v>0</v>
+      </c>
+      <c r="AO69">
+        <v>0</v>
+      </c>
+      <c r="AP69">
+        <v>0</v>
+      </c>
+      <c r="AQ69">
+        <v>0</v>
+      </c>
+      <c r="AR69">
+        <v>0</v>
+      </c>
+      <c r="AS69">
+        <v>0</v>
+      </c>
+      <c r="AT69">
+        <v>0</v>
+      </c>
+      <c r="AU69">
+        <v>0</v>
+      </c>
+      <c r="AV69">
+        <v>0</v>
+      </c>
+      <c r="AW69">
+        <v>0</v>
+      </c>
+      <c r="AX69">
+        <v>0</v>
+      </c>
+      <c r="AY69">
+        <v>0</v>
+      </c>
+      <c r="AZ69">
+        <v>0</v>
+      </c>
+      <c r="BA69">
+        <v>0</v>
+      </c>
+      <c r="BB69">
+        <v>0</v>
+      </c>
+      <c r="BC69">
+        <v>0</v>
+      </c>
+      <c r="BD69">
+        <v>0</v>
+      </c>
+      <c r="BE69">
+        <v>0</v>
+      </c>
+      <c r="BF69">
+        <v>0</v>
+      </c>
+      <c r="BG69">
+        <v>0</v>
+      </c>
+      <c r="BH69">
+        <v>0</v>
+      </c>
+      <c r="BI69">
+        <v>0</v>
+      </c>
+      <c r="BJ69">
+        <v>0</v>
+      </c>
+      <c r="BK69">
+        <v>0</v>
+      </c>
+      <c r="BL69">
+        <v>0</v>
+      </c>
+      <c r="BM69">
+        <v>0</v>
+      </c>
+      <c r="BN69">
+        <v>0</v>
+      </c>
+      <c r="BO69">
+        <v>0</v>
+      </c>
+      <c r="BP69">
+        <v>0</v>
+      </c>
+      <c r="BQ69">
+        <v>0</v>
+      </c>
+      <c r="BR69">
+        <v>0</v>
+      </c>
+      <c r="BS69">
+        <v>0</v>
+      </c>
+      <c r="BT69">
+        <v>0</v>
+      </c>
+      <c r="BU69">
+        <v>0</v>
+      </c>
+      <c r="BV69">
+        <v>0</v>
+      </c>
+      <c r="BW69">
+        <v>0</v>
+      </c>
+      <c r="BX69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <v>0</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70">
+        <v>0</v>
+      </c>
+      <c r="T70">
+        <v>0</v>
+      </c>
+      <c r="U70">
+        <v>0</v>
+      </c>
+      <c r="V70">
+        <v>0</v>
+      </c>
+      <c r="W70">
+        <v>0</v>
+      </c>
+      <c r="X70">
+        <v>0</v>
+      </c>
+      <c r="Y70">
+        <v>0</v>
+      </c>
+      <c r="Z70">
+        <v>0</v>
+      </c>
+      <c r="AA70">
+        <v>0</v>
+      </c>
+      <c r="AB70">
+        <v>0</v>
+      </c>
+      <c r="AC70">
+        <v>0</v>
+      </c>
+      <c r="AD70">
+        <v>0</v>
+      </c>
+      <c r="AE70">
+        <v>0</v>
+      </c>
+      <c r="AF70">
+        <v>0</v>
+      </c>
+      <c r="AG70">
+        <v>0</v>
+      </c>
+      <c r="AH70">
+        <v>0</v>
+      </c>
+      <c r="AI70">
+        <v>0</v>
+      </c>
+      <c r="AJ70">
+        <v>0</v>
+      </c>
+      <c r="AK70">
+        <v>0</v>
+      </c>
+      <c r="AL70">
+        <v>0</v>
+      </c>
+      <c r="AM70">
+        <v>0</v>
+      </c>
+      <c r="AN70">
+        <v>0</v>
+      </c>
+      <c r="AO70">
+        <v>0</v>
+      </c>
+      <c r="AP70">
+        <v>0</v>
+      </c>
+      <c r="AQ70">
+        <v>0</v>
+      </c>
+      <c r="AR70">
+        <v>0</v>
+      </c>
+      <c r="AS70">
+        <v>0</v>
+      </c>
+      <c r="AT70">
+        <v>0</v>
+      </c>
+      <c r="AU70">
+        <v>0</v>
+      </c>
+      <c r="AV70">
+        <v>0</v>
+      </c>
+      <c r="AW70">
+        <v>0</v>
+      </c>
+      <c r="AX70">
+        <v>0</v>
+      </c>
+      <c r="AY70">
+        <v>0</v>
+      </c>
+      <c r="AZ70">
+        <v>0</v>
+      </c>
+      <c r="BA70">
+        <v>0</v>
+      </c>
+      <c r="BB70">
+        <v>0</v>
+      </c>
+      <c r="BC70">
+        <v>0</v>
+      </c>
+      <c r="BD70">
+        <v>0</v>
+      </c>
+      <c r="BE70">
+        <v>0</v>
+      </c>
+      <c r="BF70">
+        <v>0</v>
+      </c>
+      <c r="BG70">
+        <v>0</v>
+      </c>
+      <c r="BH70">
+        <v>0</v>
+      </c>
+      <c r="BI70">
+        <v>0</v>
+      </c>
+      <c r="BJ70">
+        <v>0</v>
+      </c>
+      <c r="BK70">
+        <v>0</v>
+      </c>
+      <c r="BL70">
+        <v>0</v>
+      </c>
+      <c r="BM70">
+        <v>0</v>
+      </c>
+      <c r="BN70">
+        <v>0</v>
+      </c>
+      <c r="BO70">
+        <v>0</v>
+      </c>
+      <c r="BP70">
+        <v>0</v>
+      </c>
+      <c r="BQ70">
+        <v>0</v>
+      </c>
+      <c r="BR70">
+        <v>0</v>
+      </c>
+      <c r="BS70">
+        <v>0</v>
+      </c>
+      <c r="BT70">
+        <v>0</v>
+      </c>
+      <c r="BU70">
+        <v>0</v>
+      </c>
+      <c r="BV70">
+        <v>0</v>
+      </c>
+      <c r="BW70">
+        <v>0</v>
+      </c>
+      <c r="BX70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+      <c r="U71">
+        <v>0</v>
+      </c>
+      <c r="V71">
+        <v>0</v>
+      </c>
+      <c r="W71">
+        <v>0</v>
+      </c>
+      <c r="X71">
+        <v>0</v>
+      </c>
+      <c r="Y71">
+        <v>0</v>
+      </c>
+      <c r="Z71">
+        <v>0</v>
+      </c>
+      <c r="AA71">
+        <v>0</v>
+      </c>
+      <c r="AB71">
+        <v>0</v>
+      </c>
+      <c r="AC71">
+        <v>0</v>
+      </c>
+      <c r="AD71">
+        <v>0</v>
+      </c>
+      <c r="AE71">
+        <v>0</v>
+      </c>
+      <c r="AF71">
+        <v>0</v>
+      </c>
+      <c r="AG71">
+        <v>0</v>
+      </c>
+      <c r="AH71">
+        <v>0</v>
+      </c>
+      <c r="AI71">
+        <v>0</v>
+      </c>
+      <c r="AJ71">
+        <v>0</v>
+      </c>
+      <c r="AK71">
+        <v>0</v>
+      </c>
+      <c r="AL71">
+        <v>0</v>
+      </c>
+      <c r="AM71">
+        <v>0</v>
+      </c>
+      <c r="AN71">
+        <v>0</v>
+      </c>
+      <c r="AO71">
+        <v>0</v>
+      </c>
+      <c r="AP71">
+        <v>0</v>
+      </c>
+      <c r="AQ71">
+        <v>0</v>
+      </c>
+      <c r="AR71">
+        <v>0</v>
+      </c>
+      <c r="AS71">
+        <v>0</v>
+      </c>
+      <c r="AT71">
+        <v>0</v>
+      </c>
+      <c r="AU71">
+        <v>0</v>
+      </c>
+      <c r="AV71">
+        <v>0</v>
+      </c>
+      <c r="AW71">
+        <v>0</v>
+      </c>
+      <c r="AX71">
+        <v>0</v>
+      </c>
+      <c r="AY71">
+        <v>0</v>
+      </c>
+      <c r="AZ71">
+        <v>0</v>
+      </c>
+      <c r="BA71">
+        <v>0</v>
+      </c>
+      <c r="BB71">
+        <v>0</v>
+      </c>
+      <c r="BC71">
+        <v>0</v>
+      </c>
+      <c r="BD71">
+        <v>0</v>
+      </c>
+      <c r="BE71">
+        <v>0</v>
+      </c>
+      <c r="BF71">
+        <v>0</v>
+      </c>
+      <c r="BG71">
+        <v>0</v>
+      </c>
+      <c r="BH71">
+        <v>0</v>
+      </c>
+      <c r="BI71">
+        <v>0</v>
+      </c>
+      <c r="BJ71">
+        <v>0</v>
+      </c>
+      <c r="BK71">
+        <v>0</v>
+      </c>
+      <c r="BL71">
+        <v>0</v>
+      </c>
+      <c r="BM71">
+        <v>0</v>
+      </c>
+      <c r="BN71">
+        <v>0</v>
+      </c>
+      <c r="BO71">
+        <v>0</v>
+      </c>
+      <c r="BP71">
+        <v>0</v>
+      </c>
+      <c r="BQ71">
+        <v>0</v>
+      </c>
+      <c r="BR71">
+        <v>0</v>
+      </c>
+      <c r="BS71">
+        <v>0</v>
+      </c>
+      <c r="BT71">
+        <v>0</v>
+      </c>
+      <c r="BU71">
+        <v>0</v>
+      </c>
+      <c r="BV71">
+        <v>0</v>
+      </c>
+      <c r="BW71">
+        <v>0</v>
+      </c>
+      <c r="BX71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
+        <v>0</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72">
+        <v>0</v>
+      </c>
+      <c r="T72">
+        <v>0</v>
+      </c>
+      <c r="U72">
+        <v>0</v>
+      </c>
+      <c r="V72">
+        <v>0</v>
+      </c>
+      <c r="W72">
+        <v>0</v>
+      </c>
+      <c r="X72">
+        <v>0</v>
+      </c>
+      <c r="Y72">
+        <v>0</v>
+      </c>
+      <c r="Z72">
+        <v>0</v>
+      </c>
+      <c r="AA72">
+        <v>0</v>
+      </c>
+      <c r="AB72">
+        <v>0</v>
+      </c>
+      <c r="AC72">
+        <v>0</v>
+      </c>
+      <c r="AD72">
+        <v>0</v>
+      </c>
+      <c r="AE72">
+        <v>0</v>
+      </c>
+      <c r="AF72">
+        <v>0</v>
+      </c>
+      <c r="AG72">
+        <v>0</v>
+      </c>
+      <c r="AH72">
+        <v>0</v>
+      </c>
+      <c r="AI72">
+        <v>0</v>
+      </c>
+      <c r="AJ72">
+        <v>0</v>
+      </c>
+      <c r="AK72">
+        <v>0</v>
+      </c>
+      <c r="AL72">
+        <v>0</v>
+      </c>
+      <c r="AM72">
+        <v>0</v>
+      </c>
+      <c r="AN72">
+        <v>0</v>
+      </c>
+      <c r="AO72">
+        <v>0</v>
+      </c>
+      <c r="AP72">
+        <v>0</v>
+      </c>
+      <c r="AQ72">
+        <v>0</v>
+      </c>
+      <c r="AR72">
+        <v>0</v>
+      </c>
+      <c r="AS72">
+        <v>0</v>
+      </c>
+      <c r="AT72">
+        <v>0</v>
+      </c>
+      <c r="AU72">
+        <v>0</v>
+      </c>
+      <c r="AV72">
+        <v>0</v>
+      </c>
+      <c r="AW72">
+        <v>0</v>
+      </c>
+      <c r="AX72">
+        <v>0</v>
+      </c>
+      <c r="AY72">
+        <v>0</v>
+      </c>
+      <c r="AZ72">
+        <v>0</v>
+      </c>
+      <c r="BA72">
+        <v>0</v>
+      </c>
+      <c r="BB72">
+        <v>0</v>
+      </c>
+      <c r="BC72">
+        <v>0</v>
+      </c>
+      <c r="BD72">
+        <v>0</v>
+      </c>
+      <c r="BE72">
+        <v>0</v>
+      </c>
+      <c r="BF72">
+        <v>0</v>
+      </c>
+      <c r="BG72">
+        <v>0</v>
+      </c>
+      <c r="BH72">
+        <v>0</v>
+      </c>
+      <c r="BI72">
+        <v>0</v>
+      </c>
+      <c r="BJ72">
+        <v>0</v>
+      </c>
+      <c r="BK72">
+        <v>0</v>
+      </c>
+      <c r="BL72">
+        <v>0</v>
+      </c>
+      <c r="BM72">
+        <v>0</v>
+      </c>
+      <c r="BN72">
+        <v>0</v>
+      </c>
+      <c r="BO72">
+        <v>0</v>
+      </c>
+      <c r="BP72">
+        <v>0</v>
+      </c>
+      <c r="BQ72">
+        <v>0</v>
+      </c>
+      <c r="BR72">
+        <v>0</v>
+      </c>
+      <c r="BS72">
+        <v>0</v>
+      </c>
+      <c r="BT72">
+        <v>0</v>
+      </c>
+      <c r="BU72">
+        <v>0</v>
+      </c>
+      <c r="BV72">
+        <v>0</v>
+      </c>
+      <c r="BW72">
+        <v>0</v>
+      </c>
+      <c r="BX72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>0</v>
+      </c>
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="Q73">
+        <v>0</v>
+      </c>
+      <c r="R73">
+        <v>0</v>
+      </c>
+      <c r="S73">
+        <v>0</v>
+      </c>
+      <c r="T73">
+        <v>0</v>
+      </c>
+      <c r="U73">
+        <v>0</v>
+      </c>
+      <c r="V73">
+        <v>0</v>
+      </c>
+      <c r="W73">
+        <v>0</v>
+      </c>
+      <c r="X73">
+        <v>0</v>
+      </c>
+      <c r="Y73">
+        <v>0</v>
+      </c>
+      <c r="Z73">
+        <v>0</v>
+      </c>
+      <c r="AA73">
+        <v>0</v>
+      </c>
+      <c r="AB73">
+        <v>0</v>
+      </c>
+      <c r="AC73">
+        <v>0</v>
+      </c>
+      <c r="AD73">
+        <v>0</v>
+      </c>
+      <c r="AE73">
+        <v>0</v>
+      </c>
+      <c r="AF73">
+        <v>0</v>
+      </c>
+      <c r="AG73">
+        <v>0</v>
+      </c>
+      <c r="AH73">
+        <v>0</v>
+      </c>
+      <c r="AI73">
+        <v>0</v>
+      </c>
+      <c r="AJ73">
+        <v>0</v>
+      </c>
+      <c r="AK73">
+        <v>0</v>
+      </c>
+      <c r="AL73">
+        <v>0</v>
+      </c>
+      <c r="AM73">
+        <v>0</v>
+      </c>
+      <c r="AN73">
+        <v>0</v>
+      </c>
+      <c r="AO73">
+        <v>0</v>
+      </c>
+      <c r="AP73">
+        <v>0</v>
+      </c>
+      <c r="AQ73">
+        <v>0</v>
+      </c>
+      <c r="AR73">
+        <v>0</v>
+      </c>
+      <c r="AS73">
+        <v>0</v>
+      </c>
+      <c r="AT73">
+        <v>0</v>
+      </c>
+      <c r="AU73">
+        <v>0</v>
+      </c>
+      <c r="AV73">
+        <v>0</v>
+      </c>
+      <c r="AW73">
+        <v>0</v>
+      </c>
+      <c r="AX73">
+        <v>0</v>
+      </c>
+      <c r="AY73">
+        <v>0</v>
+      </c>
+      <c r="AZ73">
+        <v>0</v>
+      </c>
+      <c r="BA73">
+        <v>0</v>
+      </c>
+      <c r="BB73">
+        <v>0</v>
+      </c>
+      <c r="BC73">
+        <v>0</v>
+      </c>
+      <c r="BD73">
+        <v>0</v>
+      </c>
+      <c r="BE73">
+        <v>0</v>
+      </c>
+      <c r="BF73">
+        <v>0</v>
+      </c>
+      <c r="BG73">
+        <v>0</v>
+      </c>
+      <c r="BH73">
+        <v>0</v>
+      </c>
+      <c r="BI73">
+        <v>0</v>
+      </c>
+      <c r="BJ73">
+        <v>0</v>
+      </c>
+      <c r="BK73">
+        <v>0</v>
+      </c>
+      <c r="BL73">
+        <v>0</v>
+      </c>
+      <c r="BM73">
+        <v>0</v>
+      </c>
+      <c r="BN73">
+        <v>0</v>
+      </c>
+      <c r="BO73">
+        <v>0</v>
+      </c>
+      <c r="BP73">
+        <v>0</v>
+      </c>
+      <c r="BQ73">
+        <v>0</v>
+      </c>
+      <c r="BR73">
+        <v>0</v>
+      </c>
+      <c r="BS73">
+        <v>0</v>
+      </c>
+      <c r="BT73">
+        <v>0</v>
+      </c>
+      <c r="BU73">
+        <v>0</v>
+      </c>
+      <c r="BV73">
+        <v>0</v>
+      </c>
+      <c r="BW73">
+        <v>1</v>
+      </c>
+      <c r="BX73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="Q74">
+        <v>0</v>
+      </c>
+      <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="S74">
+        <v>0</v>
+      </c>
+      <c r="T74">
+        <v>0</v>
+      </c>
+      <c r="U74">
+        <v>0</v>
+      </c>
+      <c r="V74">
+        <v>0</v>
+      </c>
+      <c r="W74">
+        <v>0</v>
+      </c>
+      <c r="X74">
+        <v>0</v>
+      </c>
+      <c r="Y74">
+        <v>0</v>
+      </c>
+      <c r="Z74">
+        <v>0</v>
+      </c>
+      <c r="AA74">
+        <v>0</v>
+      </c>
+      <c r="AB74">
+        <v>0</v>
+      </c>
+      <c r="AC74">
+        <v>0</v>
+      </c>
+      <c r="AD74">
+        <v>0</v>
+      </c>
+      <c r="AE74">
+        <v>0</v>
+      </c>
+      <c r="AF74">
+        <v>0</v>
+      </c>
+      <c r="AG74">
+        <v>0</v>
+      </c>
+      <c r="AH74">
+        <v>0</v>
+      </c>
+      <c r="AI74">
+        <v>0</v>
+      </c>
+      <c r="AJ74">
+        <v>0</v>
+      </c>
+      <c r="AK74">
+        <v>0</v>
+      </c>
+      <c r="AL74">
+        <v>0</v>
+      </c>
+      <c r="AM74">
+        <v>0</v>
+      </c>
+      <c r="AN74">
+        <v>0</v>
+      </c>
+      <c r="AO74">
+        <v>0</v>
+      </c>
+      <c r="AP74">
+        <v>0</v>
+      </c>
+      <c r="AQ74">
+        <v>0</v>
+      </c>
+      <c r="AR74">
+        <v>0</v>
+      </c>
+      <c r="AS74">
+        <v>0</v>
+      </c>
+      <c r="AT74">
+        <v>0</v>
+      </c>
+      <c r="AU74">
+        <v>0</v>
+      </c>
+      <c r="AV74">
+        <v>0</v>
+      </c>
+      <c r="AW74">
+        <v>0</v>
+      </c>
+      <c r="AX74">
+        <v>0</v>
+      </c>
+      <c r="AY74">
+        <v>0</v>
+      </c>
+      <c r="AZ74">
+        <v>0</v>
+      </c>
+      <c r="BA74">
+        <v>0</v>
+      </c>
+      <c r="BB74">
+        <v>0</v>
+      </c>
+      <c r="BC74">
+        <v>0</v>
+      </c>
+      <c r="BD74">
+        <v>0</v>
+      </c>
+      <c r="BE74">
+        <v>0</v>
+      </c>
+      <c r="BF74">
+        <v>1</v>
+      </c>
+      <c r="BG74">
+        <v>0</v>
+      </c>
+      <c r="BH74">
+        <v>0</v>
+      </c>
+      <c r="BI74">
+        <v>0</v>
+      </c>
+      <c r="BJ74">
+        <v>0</v>
+      </c>
+      <c r="BK74">
+        <v>0</v>
+      </c>
+      <c r="BL74">
+        <v>0</v>
+      </c>
+      <c r="BM74">
+        <v>0</v>
+      </c>
+      <c r="BN74">
+        <v>0</v>
+      </c>
+      <c r="BO74">
+        <v>0</v>
+      </c>
+      <c r="BP74">
+        <v>0</v>
+      </c>
+      <c r="BQ74">
+        <v>0</v>
+      </c>
+      <c r="BR74">
+        <v>0</v>
+      </c>
+      <c r="BS74">
+        <v>0</v>
+      </c>
+      <c r="BT74">
+        <v>0</v>
+      </c>
+      <c r="BU74">
+        <v>0</v>
+      </c>
+      <c r="BV74">
+        <v>0</v>
+      </c>
+      <c r="BW74">
+        <v>0</v>
+      </c>
+      <c r="BX74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+      <c r="O75">
+        <v>0</v>
+      </c>
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75">
+        <v>0</v>
+      </c>
+      <c r="R75">
+        <v>0</v>
+      </c>
+      <c r="S75">
+        <v>0</v>
+      </c>
+      <c r="T75">
+        <v>0</v>
+      </c>
+      <c r="U75">
+        <v>0</v>
+      </c>
+      <c r="V75">
+        <v>0</v>
+      </c>
+      <c r="W75">
+        <v>0</v>
+      </c>
+      <c r="X75">
+        <v>0</v>
+      </c>
+      <c r="Y75">
+        <v>0</v>
+      </c>
+      <c r="Z75">
+        <v>0</v>
+      </c>
+      <c r="AA75">
+        <v>0</v>
+      </c>
+      <c r="AB75">
+        <v>0</v>
+      </c>
+      <c r="AC75">
+        <v>0</v>
+      </c>
+      <c r="AD75">
+        <v>0</v>
+      </c>
+      <c r="AE75">
+        <v>0</v>
+      </c>
+      <c r="AF75">
+        <v>0</v>
+      </c>
+      <c r="AG75">
+        <v>0</v>
+      </c>
+      <c r="AH75">
+        <v>0</v>
+      </c>
+      <c r="AI75">
+        <v>0</v>
+      </c>
+      <c r="AJ75">
+        <v>0</v>
+      </c>
+      <c r="AK75">
+        <v>0</v>
+      </c>
+      <c r="AL75">
+        <v>0</v>
+      </c>
+      <c r="AM75">
+        <v>0</v>
+      </c>
+      <c r="AN75">
+        <v>0</v>
+      </c>
+      <c r="AO75">
+        <v>0</v>
+      </c>
+      <c r="AP75">
+        <v>0</v>
+      </c>
+      <c r="AQ75">
+        <v>0</v>
+      </c>
+      <c r="AR75">
+        <v>0</v>
+      </c>
+      <c r="AS75">
+        <v>0</v>
+      </c>
+      <c r="AT75">
+        <v>0</v>
+      </c>
+      <c r="AU75">
+        <v>0</v>
+      </c>
+      <c r="AV75">
+        <v>0</v>
+      </c>
+      <c r="AW75">
+        <v>0</v>
+      </c>
+      <c r="AX75">
+        <v>0</v>
+      </c>
+      <c r="AY75">
+        <v>0</v>
+      </c>
+      <c r="AZ75">
+        <v>0</v>
+      </c>
+      <c r="BA75">
+        <v>0</v>
+      </c>
+      <c r="BB75">
+        <v>0</v>
+      </c>
+      <c r="BC75">
+        <v>0</v>
+      </c>
+      <c r="BD75">
+        <v>0</v>
+      </c>
+      <c r="BE75">
+        <v>0</v>
+      </c>
+      <c r="BF75">
+        <v>0</v>
+      </c>
+      <c r="BG75">
+        <v>0</v>
+      </c>
+      <c r="BH75">
+        <v>0</v>
+      </c>
+      <c r="BI75">
+        <v>0</v>
+      </c>
+      <c r="BJ75">
+        <v>0</v>
+      </c>
+      <c r="BK75">
+        <v>0</v>
+      </c>
+      <c r="BL75">
+        <v>0</v>
+      </c>
+      <c r="BM75">
+        <v>0</v>
+      </c>
+      <c r="BN75">
+        <v>0</v>
+      </c>
+      <c r="BO75">
+        <v>0</v>
+      </c>
+      <c r="BP75">
+        <v>0</v>
+      </c>
+      <c r="BQ75">
+        <v>0</v>
+      </c>
+      <c r="BR75">
+        <v>0</v>
+      </c>
+      <c r="BS75">
+        <v>0</v>
+      </c>
+      <c r="BT75">
+        <v>0</v>
+      </c>
+      <c r="BU75">
+        <v>0</v>
+      </c>
+      <c r="BV75">
+        <v>0</v>
+      </c>
+      <c r="BW75">
+        <v>0</v>
+      </c>
+      <c r="BX75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
+      <c r="O76">
+        <v>0</v>
+      </c>
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="Q76">
+        <v>0</v>
+      </c>
+      <c r="R76">
+        <v>0</v>
+      </c>
+      <c r="S76">
+        <v>0</v>
+      </c>
+      <c r="T76">
+        <v>0</v>
+      </c>
+      <c r="U76">
+        <v>0</v>
+      </c>
+      <c r="V76">
+        <v>0</v>
+      </c>
+      <c r="W76">
+        <v>0</v>
+      </c>
+      <c r="X76">
+        <v>0</v>
+      </c>
+      <c r="Y76">
+        <v>0</v>
+      </c>
+      <c r="Z76">
+        <v>0</v>
+      </c>
+      <c r="AA76">
+        <v>0</v>
+      </c>
+      <c r="AB76">
+        <v>0</v>
+      </c>
+      <c r="AC76">
+        <v>0</v>
+      </c>
+      <c r="AD76">
+        <v>0</v>
+      </c>
+      <c r="AE76">
+        <v>0</v>
+      </c>
+      <c r="AF76">
+        <v>0</v>
+      </c>
+      <c r="AG76">
+        <v>0</v>
+      </c>
+      <c r="AH76">
+        <v>0</v>
+      </c>
+      <c r="AI76">
+        <v>0</v>
+      </c>
+      <c r="AJ76">
+        <v>0</v>
+      </c>
+      <c r="AK76">
+        <v>0</v>
+      </c>
+      <c r="AL76">
+        <v>0</v>
+      </c>
+      <c r="AM76">
+        <v>0</v>
+      </c>
+      <c r="AN76">
+        <v>0</v>
+      </c>
+      <c r="AO76">
+        <v>0</v>
+      </c>
+      <c r="AP76">
+        <v>0</v>
+      </c>
+      <c r="AQ76">
+        <v>0</v>
+      </c>
+      <c r="AR76">
+        <v>0</v>
+      </c>
+      <c r="AS76">
+        <v>0</v>
+      </c>
+      <c r="AT76">
+        <v>0</v>
+      </c>
+      <c r="AU76">
+        <v>0</v>
+      </c>
+      <c r="AV76">
+        <v>0</v>
+      </c>
+      <c r="AW76">
+        <v>0</v>
+      </c>
+      <c r="AX76">
+        <v>0</v>
+      </c>
+      <c r="AY76">
+        <v>0</v>
+      </c>
+      <c r="AZ76">
+        <v>0</v>
+      </c>
+      <c r="BA76">
+        <v>0</v>
+      </c>
+      <c r="BB76">
+        <v>0</v>
+      </c>
+      <c r="BC76">
+        <v>0</v>
+      </c>
+      <c r="BD76">
+        <v>0</v>
+      </c>
+      <c r="BE76">
+        <v>0</v>
+      </c>
+      <c r="BF76">
+        <v>0</v>
+      </c>
+      <c r="BG76">
+        <v>0</v>
+      </c>
+      <c r="BH76">
+        <v>0</v>
+      </c>
+      <c r="BI76">
+        <v>0</v>
+      </c>
+      <c r="BJ76">
+        <v>0</v>
+      </c>
+      <c r="BK76">
+        <v>0</v>
+      </c>
+      <c r="BL76">
+        <v>0</v>
+      </c>
+      <c r="BM76">
+        <v>0</v>
+      </c>
+      <c r="BN76">
+        <v>0</v>
+      </c>
+      <c r="BO76">
+        <v>0</v>
+      </c>
+      <c r="BP76">
+        <v>0</v>
+      </c>
+      <c r="BQ76">
+        <v>0</v>
+      </c>
+      <c r="BR76">
+        <v>0</v>
+      </c>
+      <c r="BS76">
+        <v>0</v>
+      </c>
+      <c r="BT76">
+        <v>0</v>
+      </c>
+      <c r="BU76">
+        <v>0</v>
+      </c>
+      <c r="BV76">
+        <v>0</v>
+      </c>
+      <c r="BW76">
+        <v>0</v>
+      </c>
+      <c r="BX76">
         <v>0</v>
       </c>
     </row>

</xml_diff>